<commit_message>
update HkmcVehOutputAdap signal matrix add LkaLdwAdap_SignalMatrix_V4_R2.xlsx
</commit_message>
<xml_diff>
--- a/R2/02_SignalMatrix/HkmcVehicleInpAdap/HkmcVehicleInputAdap_SignalMatrix_V3.xlsx
+++ b/R2/02_SignalMatrix/HkmcVehicleInpAdap/HkmcVehicleInputAdap_SignalMatrix_V3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\00_2020\90_GitHub\0410\Veoneer\R2\02_SignalMatrix\HkmcVehicleInpAdap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21C2C69B-DD35-45F7-A5FE-4795E8B236F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA94129F-7CE8-4438-9855-123A401D417D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{51B81819-EC55-40BC-AC3D-96F7FA05F5FF}"/>
   </bookViews>
@@ -537,9 +537,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>HkmcVehicleInput_AdasISLASetReq</t>
-  </si>
-  <si>
     <t>Cx0_AdasSetReq_Default
 Cx1_AdasSetReq_Off
 Cx2_AdasSetReq_ISLW
@@ -594,26 +591,10 @@
 Cx3_SpdUT_Error_Indicator</t>
   </si>
   <si>
-    <t>HkmcVehicleInput_SpdUnitTyp</t>
-  </si>
-  <si>
-    <t>HkmcVehicleInput_Fca1stWrngSetReq</t>
-  </si>
-  <si>
     <t>CF_AVN_WarningTimingNValueSet</t>
   </si>
   <si>
     <t>USM_Fca1stWrngSetReq</t>
-  </si>
-  <si>
-    <t>Cx0_USMFca1stWSR_Default
-Cx1_USMFca1stWSR_On_Late
-Cx2_USMFca1stWSR_ON_Normal
-Cx3_USMFca1stWSR_ON_Early
-Cx4_USMFca1stWSR_Reserved
-Cx5_USMFca1stWSR_Reserved
-Cx6_USMFca1stWSR_Reserved
-Cx7_USMFca1stWSR_Invalid</t>
   </si>
   <si>
     <t>CF_AVN_NSCCCamNValueSet</t>
@@ -771,10 +752,6 @@
 Cx1_SWRCLFASS_Key_On
 Cx2_SWRCLFASS_Reserved
 Cx3_SWRCLFASS_Invalid</t>
-  </si>
-  <si>
-    <t>BitLength:10, Factor : 0.5,CLU_DisplaySpeedValue
-Cx3FF : Error</t>
   </si>
   <si>
     <t>Cx0_TurnSR_Off
@@ -1040,22 +1017,13 @@
 Cx7_AdasLkaMSR_Invalid</t>
   </si>
   <si>
-    <t>HkmcVehInput_HBA_NValueSet</t>
-  </si>
-  <si>
     <t>CF_AVN_HBANValueSet</t>
   </si>
   <si>
     <t>USM_AdasHbaSetReq</t>
   </si>
   <si>
-    <t>HkmcVehicleInput_LkaToiUnblSta</t>
-  </si>
-  <si>
     <t>MDPS_LkaToiUnblSta</t>
-  </si>
-  <si>
-    <t>HkmcVehInput_HBA_ControlMode</t>
   </si>
   <si>
     <t>CF_Gway_HBAControlMode</t>
@@ -1079,12 +1047,6 @@
     <t>U16</t>
   </si>
   <si>
-    <t>Cx0_LkaTUS_Available
-Cx1_LkaTUS_Unavailable
-Cx2_LkaTUS_Not_Used
-Cx3_LkaTUS_Error_Indicator</t>
-  </si>
-  <si>
     <t>CF_AVN_HDA_NValueSet</t>
   </si>
   <si>
@@ -1146,15 +1108,6 @@
   </si>
   <si>
     <t>4 Signals has been removed from HSCAN message CLU19 in new DBC</t>
-  </si>
-  <si>
-    <t>Cx0_ContM_HighControlMode_BCM
-Cx1_ContM_HighControlMode_HBA
-Cx2_ContM_Not_Used
-Cx3_ContM_Error_Indicator</t>
-  </si>
-  <si>
-    <t>HkmcVehicleInput_AdasFCASetReq</t>
   </si>
   <si>
     <t>Issues</t>
@@ -1217,6 +1170,64 @@
   </si>
   <si>
     <t>HkmcVehicleInput_LkaModSetReq</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>BitLength:10, Factor : 0.5,CLU_DisplaySpeedValue
+Cx3FF : Error</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cx0_ContM_HighControlMode_BCM
+Cx1_ContM_HighControlMode_HBA
+Cx2_ContM_Not_Used
+Cx3_ContM_Error_Indicator</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cx0_LkaTUS_Available
+Cx1_LkaTUS_Unavailable
+Cx2_LkaTUS_Not_Used
+Cx3_LkaTUS_Error_Indicator</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cx0_USMFca1stWSR_Default
+Cx1_USMFca1stWSR_On_Late
+Cx2_USMFca1stWSR_ON_Normal
+Cx3_USMFca1stWSR_ON_Early
+Cx4_USMFca1stWSR_Reserved
+Cx5_USMFca1stWSR_Reserved
+Cx6_USMFca1stWSR_Reserved
+Cx7_USMFca1stWSR_Invalid</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>HkmcVehicleInput_SpdUnitTyp</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>HkmcVehicleInput_Fca1stWrngSetReq</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>HkmcVehicleInput_AdasFCASetReq</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>HkmcVehInput_HBA_NValueSet</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>HkmcVehicleInput_AdasISLASetReq</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>HkmcVehicleInput_LkaToiUnblSta</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>HkmcVehInput_HBA_ControlMode</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -2740,10 +2751,10 @@
         <v>5</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>254</v>
+        <v>243</v>
       </c>
       <c r="F7" s="78" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
@@ -2779,10 +2790,10 @@
         <v>8</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>254</v>
+        <v>243</v>
       </c>
       <c r="F8" s="78" t="s">
-        <v>255</v>
+        <v>244</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
@@ -4178,10 +4189,10 @@
   <dimension ref="A1:Y93"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q8" sqref="Q8"/>
+      <selection pane="bottomRight" activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -4261,7 +4272,7 @@
         <v>4</v>
       </c>
       <c r="U1" s="76" t="s">
-        <v>251</v>
+        <v>240</v>
       </c>
       <c r="V1" s="41"/>
       <c r="W1" s="41"/>
@@ -4289,7 +4300,7 @@
         <v>17</v>
       </c>
       <c r="P2" s="40" t="s">
-        <v>135</v>
+        <v>252</v>
       </c>
       <c r="Q2" s="40" t="s">
         <v>18</v>
@@ -4298,11 +4309,11 @@
         <v>19</v>
       </c>
       <c r="S2" s="53" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="T2" s="41"/>
       <c r="U2" s="84" t="s">
-        <v>252</v>
+        <v>241</v>
       </c>
       <c r="V2" s="41"/>
       <c r="W2" s="41"/>
@@ -4330,7 +4341,7 @@
         <v>20</v>
       </c>
       <c r="P3" s="40" t="s">
-        <v>136</v>
+        <v>253</v>
       </c>
       <c r="Q3" s="40" t="s">
         <v>18</v>
@@ -4339,10 +4350,10 @@
         <v>19</v>
       </c>
       <c r="S3" s="64" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="T3" s="60" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="U3" s="84"/>
       <c r="V3" s="41"/>
@@ -4371,7 +4382,7 @@
         <v>20</v>
       </c>
       <c r="P4" s="40" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="Q4" s="40" t="s">
         <v>18</v>
@@ -4410,7 +4421,7 @@
         <v>17</v>
       </c>
       <c r="P5" s="79" t="s">
-        <v>258</v>
+        <v>247</v>
       </c>
       <c r="Q5" s="79" t="s">
         <v>18</v>
@@ -4419,7 +4430,7 @@
         <v>19</v>
       </c>
       <c r="S5" s="80" t="s">
-        <v>257</v>
+        <v>246</v>
       </c>
       <c r="T5" s="53"/>
       <c r="U5" s="84"/>
@@ -4449,7 +4460,7 @@
         <v>20</v>
       </c>
       <c r="P6" s="40" t="s">
-        <v>217</v>
+        <v>255</v>
       </c>
       <c r="Q6" s="40" t="s">
         <v>18</v>
@@ -4458,10 +4469,10 @@
         <v>19</v>
       </c>
       <c r="S6" s="64" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="T6" s="60" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="U6" s="84"/>
       <c r="V6" s="41"/>
@@ -4480,7 +4491,7 @@
         <v>20</v>
       </c>
       <c r="P7" s="66" t="s">
-        <v>123</v>
+        <v>256</v>
       </c>
       <c r="Q7" s="66" t="s">
         <v>18</v>
@@ -4489,10 +4500,10 @@
         <v>19</v>
       </c>
       <c r="S7" s="64" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="T7" s="67" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="U7" s="84"/>
     </row>
@@ -4517,7 +4528,7 @@
         <v>22</v>
       </c>
       <c r="P8" s="40" t="s">
-        <v>220</v>
+        <v>257</v>
       </c>
       <c r="Q8" s="40" t="s">
         <v>18</v>
@@ -4526,7 +4537,7 @@
         <v>19</v>
       </c>
       <c r="S8" s="53" t="s">
-        <v>228</v>
+        <v>250</v>
       </c>
       <c r="T8" s="41"/>
       <c r="U8" s="84"/>
@@ -4556,7 +4567,7 @@
         <v>23</v>
       </c>
       <c r="P9" s="40" t="s">
-        <v>222</v>
+        <v>258</v>
       </c>
       <c r="Q9" s="40" t="s">
         <v>18</v>
@@ -4631,10 +4642,10 @@
         <v>27</v>
       </c>
       <c r="S11" s="55" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="T11" s="73" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="U11" s="84"/>
       <c r="V11" s="41"/>
@@ -4658,7 +4669,7 @@
         <v>27</v>
       </c>
       <c r="S12" s="55" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="U12" s="84"/>
     </row>
@@ -4678,7 +4689,7 @@
         <v>27</v>
       </c>
       <c r="S13" s="55" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="U13" s="84"/>
     </row>
@@ -4692,13 +4703,13 @@
         <v>30</v>
       </c>
       <c r="Q14" s="68" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="R14" s="54" t="s">
         <v>27</v>
       </c>
       <c r="S14" s="55" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="U14" s="84"/>
     </row>
@@ -4709,7 +4720,7 @@
       <c r="N15" s="52"/>
       <c r="O15" s="89"/>
       <c r="P15" s="61" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Q15" s="54" t="s">
         <v>18</v>
@@ -4718,7 +4729,7 @@
         <v>27</v>
       </c>
       <c r="S15" s="55" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="U15" s="84"/>
     </row>
@@ -4738,7 +4749,7 @@
         <v>27</v>
       </c>
       <c r="S16" s="55" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="U16" s="84"/>
     </row>
@@ -4765,10 +4776,10 @@
         <v>27</v>
       </c>
       <c r="S17" s="55" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="T17" s="73" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
       <c r="U17" s="84"/>
       <c r="W17" s="62"/>
@@ -4788,7 +4799,7 @@
         <v>27</v>
       </c>
       <c r="S18" s="55" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="U18" s="84"/>
     </row>
@@ -4798,7 +4809,7 @@
       <c r="N19" s="52"/>
       <c r="O19" s="89"/>
       <c r="P19" s="68" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="Q19" s="68" t="s">
         <v>18</v>
@@ -4807,10 +4818,10 @@
         <v>27</v>
       </c>
       <c r="S19" s="65" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="T19" s="74" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
       <c r="U19" s="84"/>
     </row>
@@ -4826,7 +4837,7 @@
       <c r="N20" s="52"/>
       <c r="O20" s="89"/>
       <c r="P20" s="54" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="Q20" s="54" t="s">
         <v>18</v>
@@ -4835,7 +4846,7 @@
         <v>27</v>
       </c>
       <c r="S20" s="55" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="U20" s="84"/>
     </row>
@@ -4845,7 +4856,7 @@
       <c r="N21" s="52"/>
       <c r="O21" s="89"/>
       <c r="P21" s="61" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="Q21" s="54" t="s">
         <v>18</v>
@@ -4854,7 +4865,7 @@
         <v>27</v>
       </c>
       <c r="S21" s="65" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="U21" s="84"/>
     </row>
@@ -4873,7 +4884,7 @@
         <v>27</v>
       </c>
       <c r="S22" s="55" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="U22" s="84"/>
     </row>
@@ -4889,7 +4900,7 @@
       <c r="N23" s="52"/>
       <c r="O23" s="89"/>
       <c r="P23" s="61" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="Q23" s="54" t="s">
         <v>18</v>
@@ -4898,7 +4909,7 @@
         <v>27</v>
       </c>
       <c r="S23" s="65" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="U23" s="84"/>
     </row>
@@ -4908,7 +4919,7 @@
       <c r="N24" s="52"/>
       <c r="O24" s="89"/>
       <c r="P24" s="61" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="Q24" s="54" t="s">
         <v>18</v>
@@ -4917,7 +4928,7 @@
         <v>27</v>
       </c>
       <c r="S24" s="55" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="U24" s="84"/>
     </row>
@@ -4936,7 +4947,7 @@
         <v>27</v>
       </c>
       <c r="S25" s="55" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="U25" s="84"/>
     </row>
@@ -4955,7 +4966,7 @@
         <v>27</v>
       </c>
       <c r="S26" s="55" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="U26" s="84"/>
     </row>
@@ -4976,16 +4987,16 @@
         <v>40</v>
       </c>
       <c r="Q27" s="68" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="R27" s="54" t="s">
         <v>27</v>
       </c>
       <c r="S27" s="55" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="T27" s="73" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
       <c r="U27" s="84"/>
     </row>
@@ -5004,7 +5015,7 @@
         <v>27</v>
       </c>
       <c r="S28" s="55" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="U28" s="84"/>
     </row>
@@ -5023,7 +5034,7 @@
         <v>27</v>
       </c>
       <c r="S29" s="55" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="U29" s="84"/>
     </row>
@@ -5042,7 +5053,7 @@
         <v>27</v>
       </c>
       <c r="S30" s="55" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="U30" s="84"/>
     </row>
@@ -5061,7 +5072,7 @@
         <v>27</v>
       </c>
       <c r="S31" s="55" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="U31" s="84"/>
     </row>
@@ -5080,7 +5091,7 @@
         <v>27</v>
       </c>
       <c r="S32" s="55" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="U32" s="84"/>
     </row>
@@ -5090,7 +5101,7 @@
       <c r="N33" s="52"/>
       <c r="O33" s="89"/>
       <c r="P33" s="68" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="Q33" s="68" t="s">
         <v>31</v>
@@ -5099,10 +5110,10 @@
         <v>27</v>
       </c>
       <c r="S33" s="65" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="T33" s="73" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="U33" s="84"/>
     </row>
@@ -5123,10 +5134,10 @@
         <v>27</v>
       </c>
       <c r="S34" s="65" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="T34" s="73" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="U34" s="84"/>
     </row>
@@ -5145,10 +5156,10 @@
         <v>27</v>
       </c>
       <c r="S35" s="55" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="T35" s="73" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
       <c r="U35" s="84"/>
     </row>
@@ -5167,7 +5178,7 @@
         <v>27</v>
       </c>
       <c r="S36" s="55" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="U36" s="84"/>
     </row>
@@ -5186,7 +5197,7 @@
         <v>27</v>
       </c>
       <c r="S37" s="55" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="U37" s="84"/>
     </row>
@@ -5205,7 +5216,7 @@
         <v>27</v>
       </c>
       <c r="S38" s="55" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="U38" s="84"/>
     </row>
@@ -5224,7 +5235,7 @@
         <v>27</v>
       </c>
       <c r="S39" s="55" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="U39" s="84"/>
     </row>
@@ -5243,7 +5254,7 @@
         <v>27</v>
       </c>
       <c r="S40" s="55" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="U40" s="84"/>
     </row>
@@ -5262,7 +5273,7 @@
         <v>27</v>
       </c>
       <c r="S41" s="55" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="U41" s="84"/>
     </row>
@@ -5281,7 +5292,7 @@
         <v>27</v>
       </c>
       <c r="S42" s="59" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="U42" s="84"/>
     </row>
@@ -5291,7 +5302,7 @@
       <c r="N43" s="52"/>
       <c r="O43" s="89"/>
       <c r="P43" s="69" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="Q43" s="68" t="s">
         <v>18</v>
@@ -5300,10 +5311,10 @@
         <v>27</v>
       </c>
       <c r="S43" s="65" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="T43" s="73" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="U43" s="84"/>
     </row>
@@ -5322,7 +5333,7 @@
         <v>27</v>
       </c>
       <c r="S44" s="55" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="U44" s="84"/>
     </row>
@@ -5341,7 +5352,7 @@
         <v>27</v>
       </c>
       <c r="S45" s="55" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="U45" s="84"/>
     </row>
@@ -5360,7 +5371,7 @@
         <v>27</v>
       </c>
       <c r="S46" s="55" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="U46" s="84"/>
     </row>
@@ -5379,7 +5390,7 @@
         <v>27</v>
       </c>
       <c r="S47" s="55" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="U47" s="84"/>
     </row>
@@ -5398,7 +5409,7 @@
         <v>27</v>
       </c>
       <c r="S48" s="55" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="U48" s="84"/>
     </row>
@@ -5417,7 +5428,7 @@
         <v>27</v>
       </c>
       <c r="S49" s="55" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="U49" s="84"/>
     </row>
@@ -5427,7 +5438,7 @@
       <c r="N50" s="52"/>
       <c r="O50" s="89"/>
       <c r="P50" s="63" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="Q50" s="54" t="s">
         <v>18</v>
@@ -5436,7 +5447,7 @@
         <v>27</v>
       </c>
       <c r="S50" s="55" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="U50" s="84"/>
     </row>
@@ -5455,7 +5466,7 @@
         <v>27</v>
       </c>
       <c r="S51" s="55" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="U51" s="84"/>
     </row>
@@ -5480,7 +5491,7 @@
         <v>27</v>
       </c>
       <c r="S52" s="59" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="U52" s="84"/>
     </row>
@@ -5529,7 +5540,7 @@
         <v>114</v>
       </c>
       <c r="T54" s="73" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="U54" s="84"/>
     </row>
@@ -5558,16 +5569,16 @@
       <c r="N56" s="52"/>
       <c r="O56" s="89"/>
       <c r="P56" s="61" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q56" s="54" t="s">
+        <v>18</v>
+      </c>
+      <c r="R56" s="54" t="s">
+        <v>27</v>
+      </c>
+      <c r="S56" s="55" t="s">
         <v>133</v>
-      </c>
-      <c r="Q56" s="54" t="s">
-        <v>18</v>
-      </c>
-      <c r="R56" s="54" t="s">
-        <v>27</v>
-      </c>
-      <c r="S56" s="55" t="s">
-        <v>134</v>
       </c>
       <c r="U56" s="84"/>
     </row>
@@ -5577,7 +5588,7 @@
       <c r="N57" s="52"/>
       <c r="O57" s="89"/>
       <c r="P57" s="68" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="Q57" s="68" t="s">
         <v>18</v>
@@ -5586,10 +5597,10 @@
         <v>27</v>
       </c>
       <c r="S57" s="65" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="T57" s="73" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="U57" s="84"/>
     </row>
@@ -5599,7 +5610,7 @@
       <c r="N58" s="52"/>
       <c r="O58" s="89"/>
       <c r="P58" s="68" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="Q58" s="68" t="s">
         <v>18</v>
@@ -5608,10 +5619,10 @@
         <v>27</v>
       </c>
       <c r="S58" s="65" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="T58" s="73" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="U58" s="84"/>
     </row>
@@ -5630,7 +5641,7 @@
         <v>27</v>
       </c>
       <c r="S59" s="55" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="U59" s="84"/>
     </row>
@@ -5640,7 +5651,7 @@
       <c r="N60" s="52"/>
       <c r="O60" s="89"/>
       <c r="P60" s="68" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="Q60" s="68" t="s">
         <v>18</v>
@@ -5649,10 +5660,10 @@
         <v>27</v>
       </c>
       <c r="S60" s="65" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="T60" s="73" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="U60" s="84"/>
     </row>
@@ -5671,7 +5682,7 @@
         <v>27</v>
       </c>
       <c r="S61" s="55" t="s">
-        <v>167</v>
+        <v>248</v>
       </c>
       <c r="U61" s="84"/>
     </row>
@@ -5683,7 +5694,7 @@
         <v>106</v>
       </c>
       <c r="P62" s="61" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="Q62" s="54" t="s">
         <v>18</v>
@@ -5692,10 +5703,10 @@
         <v>27</v>
       </c>
       <c r="S62" s="55" t="s">
-        <v>139</v>
+        <v>251</v>
       </c>
       <c r="T62" s="73" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="U62" s="84"/>
     </row>
@@ -5714,7 +5725,7 @@
         <v>27</v>
       </c>
       <c r="S63" s="55" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="U63" s="84"/>
     </row>
@@ -5744,7 +5755,7 @@
         <v>116</v>
       </c>
       <c r="T64" s="73" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="U64" s="84"/>
     </row>
@@ -5782,7 +5793,7 @@
         <v>27</v>
       </c>
       <c r="S66" s="55" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="U66" s="84"/>
     </row>
@@ -5801,7 +5812,7 @@
         <v>27</v>
       </c>
       <c r="S67" s="55" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="U67" s="84"/>
       <c r="X67" s="62"/>
@@ -5821,7 +5832,7 @@
         <v>27</v>
       </c>
       <c r="S68" s="55" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="U68" s="84"/>
     </row>
@@ -5840,7 +5851,7 @@
         <v>27</v>
       </c>
       <c r="S69" s="55" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="U69" s="84"/>
     </row>
@@ -5859,7 +5870,7 @@
         <v>27</v>
       </c>
       <c r="S70" s="55" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="U70" s="84"/>
     </row>
@@ -5878,7 +5889,7 @@
         <v>27</v>
       </c>
       <c r="S71" s="55" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="U71" s="84"/>
     </row>
@@ -5897,7 +5908,7 @@
         <v>27</v>
       </c>
       <c r="S72" s="55" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="U72" s="84"/>
     </row>
@@ -5907,7 +5918,7 @@
       <c r="N73" s="52"/>
       <c r="O73" s="89"/>
       <c r="P73" s="54" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="Q73" s="54" t="s">
         <v>18</v>
@@ -5916,7 +5927,7 @@
         <v>27</v>
       </c>
       <c r="S73" s="55" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="U73" s="84"/>
     </row>
@@ -5946,7 +5957,7 @@
         <v>118</v>
       </c>
       <c r="T74" s="73" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="U74" s="84"/>
     </row>
@@ -5975,7 +5986,7 @@
       <c r="N76" s="52"/>
       <c r="O76" s="89"/>
       <c r="P76" s="61" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="Q76" s="54" t="s">
         <v>18</v>
@@ -5984,7 +5995,7 @@
         <v>27</v>
       </c>
       <c r="S76" s="55" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="U76" s="84"/>
     </row>
@@ -5994,7 +6005,7 @@
       <c r="N77" s="52"/>
       <c r="O77" s="89"/>
       <c r="P77" s="61" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="Q77" s="54" t="s">
         <v>18</v>
@@ -6003,7 +6014,7 @@
         <v>27</v>
       </c>
       <c r="S77" s="55" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="U77" s="84"/>
     </row>
@@ -6013,19 +6024,19 @@
       <c r="N78" s="52"/>
       <c r="O78" s="89"/>
       <c r="P78" s="68" t="s">
+        <v>144</v>
+      </c>
+      <c r="Q78" s="68" t="s">
+        <v>18</v>
+      </c>
+      <c r="R78" s="68" t="s">
+        <v>27</v>
+      </c>
+      <c r="S78" s="65" t="s">
         <v>148</v>
       </c>
-      <c r="Q78" s="68" t="s">
-        <v>18</v>
-      </c>
-      <c r="R78" s="68" t="s">
-        <v>27</v>
-      </c>
-      <c r="S78" s="65" t="s">
-        <v>152</v>
-      </c>
       <c r="T78" s="73" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="U78" s="84"/>
     </row>
@@ -6035,7 +6046,7 @@
       <c r="N79" s="52"/>
       <c r="O79" s="90"/>
       <c r="P79" s="68" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="Q79" s="68" t="s">
         <v>18</v>
@@ -6044,10 +6055,10 @@
         <v>27</v>
       </c>
       <c r="S79" s="65" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="T79" s="73" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="U79" s="84"/>
     </row>
@@ -6077,7 +6088,7 @@
         <v>120</v>
       </c>
       <c r="T80" s="73" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="U80" s="84"/>
     </row>
@@ -6096,7 +6107,7 @@
         <v>27</v>
       </c>
       <c r="S81" s="55" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="U81" s="84"/>
     </row>
@@ -6115,7 +6126,7 @@
         <v>27</v>
       </c>
       <c r="S82" s="55" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="U82" s="84"/>
     </row>
@@ -6134,7 +6145,7 @@
         <v>27</v>
       </c>
       <c r="S83" s="55" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="U83" s="84"/>
     </row>
@@ -6153,7 +6164,7 @@
         <v>27</v>
       </c>
       <c r="S84" s="55" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="U84" s="84"/>
     </row>
@@ -6163,7 +6174,7 @@
       <c r="N85" s="52"/>
       <c r="O85" s="89"/>
       <c r="P85" s="61" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="Q85" s="54" t="s">
         <v>18</v>
@@ -6172,7 +6183,7 @@
         <v>27</v>
       </c>
       <c r="S85" s="55" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="U85" s="84"/>
     </row>
@@ -6191,7 +6202,7 @@
         <v>27</v>
       </c>
       <c r="S86" s="55" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="U86" s="84"/>
     </row>
@@ -6210,7 +6221,7 @@
         <v>27</v>
       </c>
       <c r="S87" s="55" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="U87" s="84"/>
     </row>
@@ -6272,7 +6283,7 @@
       <c r="N90" s="52"/>
       <c r="O90" s="90"/>
       <c r="P90" s="61" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="Q90" s="54" t="s">
         <v>18</v>
@@ -6281,18 +6292,18 @@
         <v>27</v>
       </c>
       <c r="S90" s="55" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="U90" s="84"/>
     </row>
     <row r="91" spans="6:21" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="N91" s="43"/>
       <c r="O91" s="85" t="s">
+        <v>124</v>
+      </c>
+      <c r="P91" s="70" t="s">
         <v>125</v>
       </c>
-      <c r="P91" s="70" t="s">
-        <v>126</v>
-      </c>
       <c r="Q91" s="70" t="s">
         <v>18</v>
       </c>
@@ -6300,10 +6311,10 @@
         <v>27</v>
       </c>
       <c r="S91" s="71" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="T91" s="75" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="U91" s="84"/>
     </row>
@@ -6311,7 +6322,7 @@
       <c r="N92" s="43"/>
       <c r="O92" s="86"/>
       <c r="P92" s="70" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="Q92" s="70" t="s">
         <v>18</v>
@@ -6320,7 +6331,7 @@
         <v>27</v>
       </c>
       <c r="S92" s="71" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="U92" s="84"/>
     </row>
@@ -6328,7 +6339,7 @@
       <c r="N93" s="43"/>
       <c r="O93" s="87"/>
       <c r="P93" s="70" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="Q93" s="70" t="s">
         <v>18</v>
@@ -6337,7 +6348,7 @@
         <v>27</v>
       </c>
       <c r="S93" s="71" t="s">
-        <v>253</v>
+        <v>242</v>
       </c>
     </row>
   </sheetData>
@@ -6584,7 +6595,7 @@
         <v>108</v>
       </c>
       <c r="L2" s="44" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="M2" s="44" t="s">
         <v>109</v>
@@ -6774,7 +6785,7 @@
     <row r="11" spans="1:14" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="95"/>
       <c r="B11" s="46" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C11" s="42" t="s">
         <v>27</v>
@@ -6871,12 +6882,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7085,15 +7093,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AFD46AAD-E98A-4FA8-BFA3-1BCF67823CB2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{96EC4C15-7EED-4784-8F5D-530E01EF32B0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a0b74ea9-89d9-43cb-a163-e9320d483776"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="800f79bc-e7dd-46fb-9ad5-c233bb1abdf9"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -7118,18 +7138,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{96EC4C15-7EED-4784-8F5D-530E01EF32B0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AFD46AAD-E98A-4FA8-BFA3-1BCF67823CB2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a0b74ea9-89d9-43cb-a163-e9320d483776"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="800f79bc-e7dd-46fb-9ad5-c233bb1abdf9"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>